<commit_message>
Updated Sprint backlog and product backlog
1) updated descriptions
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog-3.xlsx
+++ b/documentation/Product Backlog-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c751dba731cb2a1/Documents/UWG/2024/Software Engineering 2/Inventory Manager Project/SE2Project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\SE2Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{CAE62280-1A45-4442-B0DA-5650FC968AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8CD12CC-61D1-4145-B75D-3F4199340303}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EACB34F-DD02-444F-A09B-44B4CA9A1888}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21540" yWindow="-26540" windowWidth="29400" windowHeight="22900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21540" yWindow="-26535" windowWidth="29400" windowHeight="22905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Priority</t>
   </si>
@@ -68,9 +57,6 @@
     <t>able to add new employees</t>
   </si>
   <si>
-    <t>Add New Raw Material</t>
-  </si>
-  <si>
     <t>If there are no raw materials, we can't produce products</t>
   </si>
   <si>
@@ -86,15 +72,9 @@
     <t>If there are no products, we can't make money</t>
   </si>
   <si>
-    <t>View Number of Raw Materials</t>
-  </si>
-  <si>
     <t>I know when to order more materials</t>
   </si>
   <si>
-    <t>View Number of Products</t>
-  </si>
-  <si>
     <t>I know how much product I'm able to sale</t>
   </si>
   <si>
@@ -104,15 +84,9 @@
     <t>I know what raw materials I need for a specific product</t>
   </si>
   <si>
-    <t>Create Order</t>
-  </si>
-  <si>
     <t>Complete Order</t>
   </si>
   <si>
-    <t>If we can't sell products, we won't have any cash</t>
-  </si>
-  <si>
     <t>Remove Raw Material</t>
   </si>
   <si>
@@ -192,6 +166,18 @@
   </si>
   <si>
     <t>see how long it takes to produce a product</t>
+  </si>
+  <si>
+    <t>Add Raw Material</t>
+  </si>
+  <si>
+    <t>View Raw Material details</t>
+  </si>
+  <si>
+    <t>View Product details</t>
+  </si>
+  <si>
+    <t>We can fullfill our duty and make customers happy</t>
   </si>
 </sst>
 </file>
@@ -266,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -278,6 +264,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,20 +545,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="153.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="153.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -599,7 +586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -613,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -621,13 +608,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -635,13 +622,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -649,13 +636,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -663,13 +650,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -677,13 +664,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -691,13 +678,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -705,25 +692,27 @@
         <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -731,13 +720,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -745,13 +734,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>3</v>
       </c>
@@ -759,55 +748,55 @@
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="7" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>3</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -815,27 +804,27 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>6</v>
       </c>
@@ -843,13 +832,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>6</v>
       </c>
@@ -857,13 +846,13 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>6</v>
       </c>
@@ -871,27 +860,27 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>6</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -899,40 +888,26 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>51</v>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:XFD1048576">
-    <sortCondition ref="A2:A1048576"/>
+  <sortState ref="A2:XFD1048575">
+    <sortCondition ref="A2:A1048575"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>